<commit_message>
finalized the draft list of WPs inputs
</commit_message>
<xml_diff>
--- a/src/databases/WP1_BoM.xlsx
+++ b/src/databases/WP1_BoM.xlsx
@@ -1,26 +1,83 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="22905"/>
+  <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="100" windowWidth="14800" windowHeight="8020"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="device" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="122211" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <t>OEC type</t>
+  </si>
+  <si>
+    <t>technlogy type</t>
+  </si>
+  <si>
+    <t>seabed fixed</t>
+  </si>
+  <si>
+    <t>wave</t>
+  </si>
+  <si>
+    <t>length [m]</t>
+  </si>
+  <si>
+    <t>height [m]</t>
+  </si>
+  <si>
+    <t>width [m]</t>
+  </si>
+  <si>
+    <t>drymass [kg]</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -41,13 +98,30 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="9">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -341,13 +415,70 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="3" max="3" width="13.6640625" customWidth="1"/>
+    <col min="7" max="7" width="12" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>100</v>
+      </c>
+      <c r="E2">
+        <v>8</v>
+      </c>
+      <c r="F2">
+        <v>8</v>
+      </c>
+      <c r="G2">
+        <v>150000</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
debug sched ongoing 2
</commit_message>
<xml_diff>
--- a/src/databases/WP1_BoM.xlsx
+++ b/src/databases/WP1_BoM.xlsx
@@ -115,7 +115,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -431,7 +431,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -487,12 +487,12 @@
         <v>150000</v>
       </c>
       <c r="H2" s="2">
-        <v>43101</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>